<commit_message>
Changes in the description of the functions
</commit_message>
<xml_diff>
--- a/Documents/V-Cycle Process/V_Cycle Process Script.xlsx
+++ b/Documents/V-Cycle Process/V_Cycle Process Script.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edgar\Desktop\AEP_Continental\Presentaciones\Papeleo\V-Cycle Process\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edgar\Desktop\Workspace\WiLi\Documents\V-Cycle Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13860" windowHeight="5085" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19245" windowHeight="8280" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="V-Cycle" sheetId="2" r:id="rId1"/>
@@ -2008,7 +2008,9 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="C2:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2623,8 +2625,8 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="C2:E25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>